<commit_message>
add legends as freeze panes
</commit_message>
<xml_diff>
--- a/Tables/Supp Table 1 - FullGoDensityLocality.xlsx
+++ b/Tables/Supp Table 1 - FullGoDensityLocality.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\CamocoManuscript\Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\VBOXSVR\rob\Documents\CamocoManuscript\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3334,7 +3334,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Full gene ontology term density and locality p-values.</t>
+      <t xml:space="preserve">Full gene ontology term density and locality p-values. </t>
     </r>
     <r>
       <rPr>
@@ -3344,8 +3344,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">
-Density and locality scores were measured between genes within each GO term. Subnetwork p-values were generated for both density and locality by comparing each term’s metric to 1,000 randomized gene sets of the same size. The "Number of Network Genes in GO Terms" indicates the intersect between genes present in the network and genes annotated to a GO term.
+      <t xml:space="preserve">Density and locality scores were measured between genes within each GO term. Subnetwork p-values were generated for both density and locality by comparing each term’s metric to 1,000 randomized gene sets of the same size. The "Number of Network Genes in GO Terms" indicates the intersect between genes present in the network and genes annotated to a GO term. Supports Table 1.
 </t>
     </r>
   </si>
@@ -38798,5 +38797,6 @@
     <mergeCell ref="A1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>